<commit_message>
Window closing issue solved
</commit_message>
<xml_diff>
--- a/data/test_results.xlsx
+++ b/data/test_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/firefly-2-houses-on-1-spectacular-property/HA-321126404</t>
+          <t>https://www.varoom.com/property/agriturismo-marano/EP-30538840</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/spire-apartments-by-barsala/BC-10089643</t>
+          <t>https://www.varoom.com/property/residence-inn-indianapolis-fishers/BC-269249</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/the-home-collection-600-hermitage-road/EP-96200494</t>
+          <t>https://www.varoom.com/property/stone-soup-inn/EP-3852352</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -538,6 +538,36 @@
         <v>1</v>
       </c>
       <c r="F4" t="inlineStr">
+        <is>
+          <t>The Property in the www.varoom.com is Available in the Specified date range</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/comfort-inn-suites-fishers-indianapolis/BC-183994</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>The Property in the www.varoom.com is Available in the Specified date range</t>
         </is>

</xml_diff>

<commit_message>
Dynamic Tiles Fetching implemented
</commit_message>
<xml_diff>
--- a/data/test_results.xlsx
+++ b/data/test_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/agriturismo-marano/EP-30538840</t>
+          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,7 +479,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The Property in the www.varoom.com is Available in the Specified date range</t>
+          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/residence-inn-indianapolis-fishers/BC-269249</t>
+          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>The Property in the www.varoom.com is Available in the Specified date range</t>
+          <t>The property 'Morris Villa' is Available in the specified date range.</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/stone-soup-inn/EP-3852352</t>
+          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>The Property in the www.varoom.com is Available in the Specified date range</t>
+          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/comfort-inn-suites-fishers-indianapolis/BC-183994</t>
+          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -569,7 +569,607 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The Property in the www.varoom.com is Available in the Specified date range</t>
+          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>The property 'Morris Villa' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>The property 'Morris Villa' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>The property 'Morris Villa' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Location and Date Range added in the comment section
</commit_message>
<xml_diff>
--- a/data/test_results.xlsx
+++ b/data/test_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
+          <t>https://www.varoom.com/property/anurra1-domus-de-janas/BC-4871160</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,11 +475,11 @@
         </is>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
+          <t>The property 'Anurra1-Domus de Janas' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
+          <t>https://www.varoom.com/property/nice-apartment-for-5-guests-with-tv-terrace-and-pets-allowed/EP-27689065</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,11 +505,11 @@
         </is>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>The property 'Morris Villa' is Available in the specified date range.</t>
+          <t>The property 'Nice apartment for 5 guests with TV, terrace and pets allowed' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
+          <t>https://www.varoom.com/property/holiday-home-isola-rossa/BC-6119796</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -535,11 +535,11 @@
         </is>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Holiday Home Isola Rossa' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
+          <t>https://www.varoom.com/property/costa-paradiso-resort/EP-102231382</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -565,11 +565,11 @@
         </is>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+          <t>The property 'Costa Paradiso Resort' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+          <t>https://www.varoom.com/property/locazione-turistica-scalitti-by-interhome/BC-3551349</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -595,11 +595,11 @@
         </is>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+          <t>The property 'Locazione Turistica Scalitti by Interhome' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+          <t>https://www.varoom.com/property/isola-rossa-borgo-mare-agenzia-isola-rossa/EP-11703078</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -625,11 +625,11 @@
         </is>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Isola Rossa Borgo Mare - Agenzia Isola Rossa' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
+          <t>https://www.varoom.com/property/walk-to-the-beach-from-your-cottage-apartment-set-in-wild-rural-sardinia/BC-3887684</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -655,11 +655,11 @@
         </is>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
+          <t>The property 'Walk To The Beach From Your Cottage-Apartment Set In Wild, Rural Sardinia' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
+          <t>https://www.varoom.com/property/gravina-resort-apartments/EP-5175840</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -685,11 +685,11 @@
         </is>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>The property 'Morris Villa' is Available in the specified date range.</t>
+          <t>The property 'Gravina Resort &amp; Apartments' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
+          <t>https://www.varoom.com/property/affittimoderni-isola-rossa-borgo/BC-4824656</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -715,11 +715,11 @@
         </is>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Affittimoderni Isola Rossa Borgo' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
+          <t>https://www.varoom.com/property/residence-with-pool-in-isola-rossa/EP-100779242</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -745,11 +745,11 @@
         </is>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+          <t>The property 'Residence with pool in Isola Rossa' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+          <t>https://www.varoom.com/property/cottage-apartment-in-rural-sardinia-with-sun-sea-and-sand/BC-3765161</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -775,11 +775,11 @@
         </is>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+          <t>The property 'Cottage-Apartment In Rural Sardinia With Sun, Sea And Sand' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+          <t>https://www.varoom.com/property/villa-rocce-rosse-costa-paradiso/EP-93506023</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -805,11 +805,11 @@
         </is>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Villa Rocce Rosse Costa Paradiso' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
+          <t>https://www.varoom.com/property/il-boschetto-dei-corbezzoli-villetta-3/BC-5288835</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -835,11 +835,11 @@
         </is>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
+          <t>The property 'Il Boschetto dei Corbezzoli villetta 3' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
+          <t>https://www.varoom.com/property/apartment-with-stunning-views/EP-96818551</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -865,11 +865,11 @@
         </is>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>The property 'Morris Villa' is Available in the specified date range.</t>
+          <t>The property 'Apartment With Stunning Views' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
+          <t>https://www.varoom.com/property/costa-paradiso-villaggio-tamerici/BC-1065581</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -895,11 +895,11 @@
         </is>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Costa Paradiso Villaggio Tamerici' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
+          <t>https://www.varoom.com/property/villetta-dei-ginepri-costa-paradiso/EP-94632555</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -925,11 +925,11 @@
         </is>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+          <t>The property 'Villetta dei Ginepri Costa Paradiso' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+          <t>https://www.varoom.com/property/il-boschetto-dei-corbezzoli-villetta-2/BC-5283284</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -955,11 +955,11 @@
         </is>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+          <t>The property 'Il Boschetto dei Corbezzoli Villetta 2' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+          <t>https://www.varoom.com/property/isola-rossa-apartment-with-breathtaking-sea-view/EP-96814262</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -985,11 +985,11 @@
         </is>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Isola Rossa Apartment With Breathtaking sea View' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/home-at-lake-junaluska-for-you-to-enjoy-this-winter-and-all-seasons-n/HA-321461826</t>
+          <t>https://www.varoom.com/property/scoglio-a-costa-paradiso/BC-3898644</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1015,11 +1015,11 @@
         </is>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>The property 'HOME AT LAKE JUNALUSKA FOR YOU TO ENJOY this WINTER and All SEASONS!n' is Available in the specified date range.</t>
+          <t>The property 'Scoglio a Costa Paradiso' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/morris-villa/BC-8294306</t>
+          <t>https://www.varoom.com/property/fronte-mare/BC-2492992</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1045,11 +1045,11 @@
         </is>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>The property 'Morris Villa' is Available in the specified date range.</t>
+          <t>The property 'Fronte Mare' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/lambuth-inn-at-lake-junaluska/EP-11898762</t>
+          <t>https://www.varoom.com/property/apartment-with-swimming-pool-in-trinit-d-agultu-e-vignola/BC-2469706</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1075,11 +1075,11 @@
         </is>
       </c>
       <c r="E22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>The property 'Lambuth Inn at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Apartment with Swimming Pool in Trinit d Agultu e Vignola' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/junaluska-lake-lake/HA-3211431838</t>
+          <t>https://www.varoom.com/property/central-apartment-irina-with-terrace/BC-2192182</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1105,11 +1105,11 @@
         </is>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>The property 'Junaluska lake-lake' is Available in the specified date range.</t>
+          <t>The property 'Central apartment Irina with terrace' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/serenity-hillside-lower/BC-8145207</t>
+          <t>https://www.varoom.com/property/camera-con-bagno-isola-rossa-paduledda/BC-8957107</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1135,11 +1135,11 @@
         </is>
       </c>
       <c r="E24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>The property 'Serenity Hillside Lower' is Available in the specified date range.</t>
+          <t>The property 'Camera con bagno Isola Rossa, Paduledda' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/the-terrace-at-lake-junaluska/EP-1604491</t>
+          <t>https://www.varoom.com/property/appartamento-isola-rossa-paduledda/BC-8879596</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1165,11 +1165,371 @@
         </is>
       </c>
       <c r="E25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>The property 'The Terrace at Lake Junaluska' is Available in the specified date range.</t>
+          <t>The property 'Appartamento Isola Rossa, Paduledda' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/sweet-costa-paradiso-splendida-vista-mare/BC-8834419</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>The property 'Sweet Costa Paradiso splendida vista mare' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/appartamento-vista-mare-via-tinnari/BC-8849180</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>The property 'Appartamento Vista Mare via Tinnari' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/emanuele-villetta-con-ampio-giardino-piscina-condizionatori-caldo-freddo/BC-7890193</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>The property 'Emanuele Villetta con Ampio Giardino Piscina CONDIZIONATORI CALDO FREDDO' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/costa-paradiso-comprensorio-in-totale-relax/BC-7635836</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>The property 'Costa paradiso comprensorio in totale relax' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/dream-isola-rossa/BC-7220073</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>The property 'Dream Isola Rossa' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/stazzo-jana/BC-11063229</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>The property 'Stazzo Jana' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/anurra1-domus-de-janas/BC-4871160</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>The property 'Anurra1-Domus de Janas' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/nice-apartment-for-5-guests-with-tv-terrace-and-pets-allowed/EP-27689065</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>The property 'Nice apartment for 5 guests with TV, terrace and pets allowed' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/holiday-home-isola-rossa/BC-6119796</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>The property 'Holiday Home Isola Rossa' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/costa-paradiso-resort/EP-102231382</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>The property 'Costa Paradiso Resort' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/locazione-turistica-scalitti-by-interhome/BC-3551349</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>The property 'Locazione Turistica Scalitti by Interhome' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/isola-rossa-borgo-mare-agenzia-isola-rossa/EP-11703078</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>The property 'Isola Rossa Borgo Mare - Agenzia Isola Rossa' is Unavailable in the specified date range. | Location: Shawnview, Dates: 2025-02-01 to 2025-02-04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Comment section modified for more professional info structure
</commit_message>
<xml_diff>
--- a/data/test_results.xlsx
+++ b/data/test_results.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/condo-with-exquisite-view-over-golf-course-free-wifi-netflix-golf-nelson-bay-beaches-boating-and-fis/HA-1309065646</t>
+          <t>https://www.varoom.com/property/beautiful-house-in-mansfield/HA-3214239599</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,7 +479,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The property 'Condo with Exquisite View over Golf Course - FREE Wifi - Netflix - Golf - Nelson Bay - Beaches - Boating and Fishing' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Beautiful House in Mansfield' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/hightide-luxury-apartment-almost-on-the-beach/BC-9629423</t>
+          <t>https://www.varoom.com/property/newly-constructed-mansfield-home-with-fenced-yard/BC-8480246</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>The property 'HighTide- luxury apartment, almost on the beach.' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Newly Constructed Mansfield Home with Fenced Yard!' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/wanderers-retreat-port-stephens/EP-9625723</t>
+          <t>https://www.varoom.com/property/newly-constructed-mansfield-home-w-fenced-yard/EP-93205463</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>The property 'Wanderers Retreat Port Stephens' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Newly Constructed Mansfield Home w/Fenced Yard!' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/ingenia-holidays-soldiers-point/BC-1559907</t>
+          <t>https://www.varoom.com/property/stylish-modern-house-in-mansfield/HA-3214239622</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The property 'Ingenia Holidays Soldiers Point' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Stylish Modern House in Mansfield' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/ingenia-holidays-soldiers-point/EP-12829777</t>
+          <t>https://www.varoom.com/property/covered-patio-and-large-yard-mansfield-home/BC-10869407</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>The property 'Ingenia Holidays Soldiers Point' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Covered Patio and Large yard Mansfield Home' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/the-boathouse-resort-luxury-apartments/BC-2862382</t>
+          <t>https://www.varoom.com/property/mansfield-home-w-private-yard-covered-patio/EP-99482582</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>The property 'The Boathouse Resort Luxury Apartments' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Mansfield Home w/Private Yard &amp; Covered Patio!' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/ingenia-holidays-one-mile-beach/EP-9625634</t>
+          <t>https://www.varoom.com/property/beautiful-5bd-3ba-near-bld-waterpark-at-t-stadium/HA-3212396444</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>The property 'Ingenia Holidays One Mile Beach' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Beautiful 5BD/3BA Near BLD/Waterpark/AT&amp;T Stadium' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/casablanca-enchanted-cottage/BC-808531</t>
+          <t>https://www.varoom.com/property/private-pool-w-full-amenities-by-bld-joe-pool-lk/BC-6383743</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>The property 'Casablanca Enchanted Cottage' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'PRIVATE POOL w/Full Amenities by BLD &amp; Joe Pool LK' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/lemon-tree-passage-motel/EP-22258483</t>
+          <t>https://www.varoom.com/property/holiday-inn-express-suites-mansfield-an-ihg-hotel/EP-1723202</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -719,7 +719,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>The property 'Lemon Tree Passage Motel' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Holiday Inn Express &amp; Suites Mansfield, an IHG Hotel' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/casablanca-penthouse-loft-landmark-518/BC-2152919</t>
+          <t>https://www.varoom.com/property/amazing-views-nature-3-porches-wi-fi-secluded-5mi-to-downtown-dine-shop/HA-3213240954</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>The property 'Casablanca Penthouse Loft - Landmark 518' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Amazing Views 🕊️Nature 3 Porches ⚡️Wi-fi Secluded .5mi to downtown dine/shop' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/anchorage-port-stephens/EP-522338</t>
+          <t>https://www.varoom.com/property/grand-home-comfort-for-everyone/BC-13224292</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>The property 'Anchorage Port Stephens' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Grand home - Comfort for everyone' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/the-fog-getaway-by-tiny-away/BC-12052705</t>
+          <t>https://www.varoom.com/property/best-western-plus-mansfield-inn-suites/EP-1829967</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>The property 'The Fog Getaway by Tiny Away' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Best Western Plus Mansfield Inn &amp; Suites' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/bannisters-port-stephens/EP-27355893</t>
+          <t>https://www.varoom.com/property/newly-constructed-mansfield-home-w-fenced-yard/HA-1219685632</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>The property 'Bannisters Port Stephens' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Newly Constructed Mansfield Home w/Fenced Yard!' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/ingenia-holidays-one-mile-beach/BC-1001856</t>
+          <t>https://www.varoom.com/property/the-estate-home/BC-12251366</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>The property 'Ingenia Holidays One Mile Beach' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'The Estate Home' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/oaks-port-stephens-pacific-blue-resort/EP-1773945</t>
+          <t>https://www.varoom.com/property/fairfield-inn-suites-by-marriott-dallas-mansfield/EP-2516425</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>The property 'Oaks Port Stephens Pacific Blue Resort' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Fairfield Inn &amp; Suites by Marriott Dallas Mansfield' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/big4-karuah-jetty-holiday-park/BC-777247</t>
+          <t>https://www.varoom.com/property/mansfield-home-w-private-yard-covered-patio/HA-1219878395</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>The property 'BIG4 Karuah Jetty Holiday Park' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Mansfield Home w/Private Yard &amp; Covered Patio!' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/corlette-palms-motor-inn/EP-9626388</t>
+          <t>https://www.varoom.com/property/brand-new-smart-home/BC-12224186</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>The property 'Corlette Palms Motor Inn' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Brand New Smart Home' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/condo-105-horizons-golf-resort-salamander-bay-nsw/BC-3403078</t>
+          <t>https://www.varoom.com/property/comfort-inn-suites-mansfield/EP-807999</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>The property 'Condo 105 @ Horizons Golf Resort - Salamander Bay NSW' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Comfort Inn &amp; Suites Mansfield' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/landmark-resort/BC-412295</t>
+          <t>https://www.varoom.com/property/enjoy-resort-style-luxury-accommodations-at-the-estate-home/HA-1217682575</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>The property 'Landmark Resort' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'ENJOY RESORT STYLE LUXURY ACCOMMODATIONS AT THE ESTATE HOME' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/wanderers-retreat/BC-793503</t>
+          <t>https://www.varoom.com/property/holiday-inn-express-hotel-suites-mansfield-an-ihg-hotel/BC-184861</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>The property 'Wanderers Retreat' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Holiday Inn Express Hotel &amp; Suites Mansfield, an IHG Hotel' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/mantra-nelson-bay/BC-323370</t>
+          <t>https://www.varoom.com/property/hampton-inn-suites-mansfield/EP-2246519</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>The property 'Mantra Nelson Bay' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Hampton Inn &amp; Suites Mansfield' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/australian-motor-home-tourist-park-twelve-mile-creek/BC-1469873</t>
+          <t>https://www.varoom.com/property/large-comfy-4br-retreat-great-location-fam-group/HA-3213151814</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>The property 'Australian Motor Home Tourist Park Twelve Mile Creek' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Large Comfy 4BR Retreat/Great Location ~Fam/Group' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/sunset-vine-at-wonganella-estate-2-by-tiny-away/BC-11050371</t>
+          <t>https://www.varoom.com/property/best-western-plus-mansfield-inn-and-suites/BC-254822</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>The property 'Sunset Vine at Wonganella Estate 2 by Tiny Away' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'Best Western Plus Mansfield Inn and Suites' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.varoom.com/property/salt-at-shoal-bay/BC-3178298</t>
+          <t>https://www.varoom.com/property/la-quinta-inn-suites-by-wyndham-mansfield-tx/EP-1844878</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>The property 'Salt at Shoal Bay' is Available in the specified date range. | Location: Port Steven, Dates: 2025-01-22 to 2025-01-23</t>
+          <t>The property 'La Quinta Inn &amp; Suites by Wyndham Mansfield TX' is Available in the specified date range. | **Location:** West Debbieton | **Date Range:** Check-in: 2025-01-25, Check-out: 2025-01-30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Testing based on REAMDE file done!
</commit_message>
<xml_diff>
--- a/data/test_results.xlsx
+++ b/data/test_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1173,6 +1173,726 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/gorgeous-loft-style-house-w-luxury-charm-comfort/HA-3212129747</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>The property '* Gorgeous Loft Style House w/Luxury, Charm, &amp; Comfort *' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/nice-bedroom-next-fells-point/BC-4875257</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>The property 'Nice bedroom next fells point' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/1840s-carrollton-inn/EP-4238812</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>The property '1840s Carrollton Inn' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/rollingside-guest-suite/HA-3212133687</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>The property 'Rollingside Guest Suite' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/chic-3-bedroom-house-in-baltimore/BC-12836036</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>The property 'Chic 3 Bedroom house in Baltimore' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/entire-unit-5min-to-m-tbank-camden-yards/EP-78004082</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>The property 'Entire Unit-5min to M&amp;TBank Camden Yards' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/glen-burnie-escape-pet-friendly-with-easy-access-to-multiple-attractions/HA-3213843374</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>The property 'Glen Burnie Escape - Pet friendly with easy access to multiple attractions.' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/fells-point-charm-doubled/BC-10671028</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>The property 'Fells Point Charm Doubled!' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/room-in-guest-room-twin-bunk-style-bedroom-close-to-downtown/EP-84610916</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>The property 'Room in Guest Room - Twin Bunk-style Bedroom Close to Downtown' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/big-3-story-house-near-stadiums-aquarium-museums-5-bedrooms-parking/HA-3213607613</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>The property 'Big 3 story house near stadiums, aquarium, museums, 5 bedrooms, parking' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/huge-downtown-baltimore-home-with-parking/BC-13221476</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>The property 'Huge Downtown Baltimore home with parking' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/room-in-guest-room-cozy-bedroom-close-to-downtown/EP-84610923</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>The property 'Room in Guest Room - Cozy Bedroom Close to Downtown' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/blue-house-in-hampden/HA-3213840308</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>The property 'Blue House in Hampden' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/home-away-from-home/BC-12692682</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>The property 'Home away from home!' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/guesthouse-by-good-neighbor/EP-96404669</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>The property 'guesthouse by good neighbor' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/cozy-1-bedroom-with-ac-and-wifi-in-marvelous-baltimore/HA-3214161410</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>The property 'Cozy 1-bedroom with AC and WiFi in marvelous Baltimore.' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/entire-house-king-bed-near-downtown-free-parking/BC-12825912</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>The property 'Entire House King Bed near Downtown Free Parking' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/four-seasons-hotel-baltimore/EP-4603198</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>The property 'Four Seasons Hotel Baltimore' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/fed-hill-luxe-with-harbor-view-rooftop-deck-parking-ev/HA-3214162843</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>The property 'Fed Hill Luxe with Harbor View Rooftop Deck, Parking &amp; EV' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/rachael-s-dowry-bed-and-breakfast/BC-529548</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>The property 'Rachael's Dowry Bed and Breakfast' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/roost-baltimore/EP-95348917</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>The property 'ROOST Baltimore' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/tiny-house-24-7-no-contact-self-check-in-bwi-area/HA-3214225097</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>The property 'Tiny House 24/7 No Contact Self Check-In BWI area' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/1840s-carrollton-inn/BC-1186462</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>The property '1840s Carrollton Inn' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>www.varoom.com</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.varoom.com/property/hotel-revival-baltimore/EP-28314</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Property available in date range</t>
+        </is>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>The property 'Hotel Revival Baltimore' is Available in the specified date range. | **Location:** Cookside | **Date Range:** Check-in: 2025-02-09, Check-out: 2025-02-10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>